<commit_message>
Gemini returning invalid JSON fixed
</commit_message>
<xml_diff>
--- a/normalized_inputs/class_ENGINEERING/extracted_offline_sheet.xlsx
+++ b/normalized_inputs/class_ENGINEERING/extracted_offline_sheet.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ENGINEERING" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="engineering" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM23"/>
+  <dimension ref="A1:AM27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,11 +631,11 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -645,12 +645,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -660,22 +660,22 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -685,27 +685,27 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
@@ -715,47 +715,47 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
@@ -770,17 +770,17 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK2" t="n">
@@ -795,18 +795,18 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>274600</v>
+        <v>281600</v>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -816,12 +816,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -831,17 +831,17 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -866,17 +866,17 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -886,17 +886,17 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
@@ -911,22 +911,22 @@
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
@@ -936,29 +936,29 @@
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK3" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AL3" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AM3" t="n">
         <v>0</v>
@@ -966,18 +966,18 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>254000</v>
+        <v>283800</v>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -987,32 +987,32 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -1027,17 +1027,17 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -1047,42 +1047,42 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
@@ -1092,12 +1092,12 @@
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
@@ -1112,24 +1112,24 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK4" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AL4" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AM4" t="n">
         <v>0</v>
@@ -1137,14 +1137,14 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>258900</v>
+        <v>271200</v>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -1158,17 +1158,17 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -1198,17 +1198,17 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -1216,7 +1216,11 @@
           <t>D</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr"/>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
       <c r="V5" t="inlineStr">
         <is>
           <t>B</t>
@@ -1224,32 +1228,32 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
@@ -1259,12 +1263,12 @@
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
@@ -1274,17 +1278,17 @@
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
@@ -1293,29 +1297,29 @@
         </is>
       </c>
       <c r="AK5" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AL5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="AM5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>274200</v>
+        <v>269200</v>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1325,12 +1329,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1340,27 +1344,27 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -1375,87 +1379,87 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
@@ -1464,10 +1468,10 @@
         </is>
       </c>
       <c r="AK6" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AM6" t="n">
         <v>0</v>
@@ -1475,18 +1479,18 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>258500</v>
+        <v>273000</v>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1496,22 +1500,22 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1521,57 +1525,37 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -1581,32 +1565,32 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
@@ -1621,43 +1605,43 @@
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK7" t="n">
         <v>17</v>
       </c>
       <c r="AL7" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="AM7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>265700</v>
+        <v>268600</v>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1667,22 +1651,22 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1697,12 +1681,12 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -1712,47 +1696,47 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
@@ -1762,18 +1746,22 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr"/>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">
@@ -1783,12 +1771,12 @@
       </c>
       <c r="AG8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
@@ -1798,33 +1786,33 @@
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK8" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AL8" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AM8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>259300</v>
+        <v>271800</v>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1834,12 +1822,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1849,22 +1837,22 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1874,7 +1862,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1884,32 +1872,32 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1924,37 +1912,37 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AH9" t="inlineStr">
@@ -1964,12 +1952,12 @@
       </c>
       <c r="AI9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK9" t="n">
@@ -1984,23 +1972,23 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>260200</v>
+        <v>900447</v>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -2010,37 +1998,37 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -2050,7 +2038,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -2060,12 +2048,12 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
@@ -2075,90 +2063,94 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="AG10" t="inlineStr"/>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AI10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK10" t="n">
         <v>16</v>
       </c>
       <c r="AL10" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AM10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>267300</v>
+        <v>265100</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2167,12 +2159,12 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -2182,17 +2174,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -2202,17 +2194,17 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -2222,52 +2214,52 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
@@ -2282,7 +2274,7 @@
       </c>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF11" t="inlineStr">
@@ -2292,29 +2284,29 @@
       </c>
       <c r="AG11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AH11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AI11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK11" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AL11" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AM11" t="n">
         <v>0</v>
@@ -2322,43 +2314,43 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>275600</v>
+        <v>286000</v>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -2383,7 +2375,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -2393,12 +2385,12 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -2408,7 +2400,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -2423,22 +2415,22 @@
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
@@ -2448,12 +2440,12 @@
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF12" t="inlineStr">
@@ -2463,7 +2455,7 @@
       </c>
       <c r="AG12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AH12" t="inlineStr">
@@ -2473,19 +2465,19 @@
       </c>
       <c r="AI12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK12" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AL12" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AM12" t="n">
         <v>0</v>
@@ -2493,18 +2485,18 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>275700</v>
+        <v>280400</v>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -2514,67 +2506,67 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
@@ -2584,12 +2576,12 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
@@ -2604,12 +2596,12 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
@@ -2619,12 +2611,12 @@
       </c>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AE13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AF13" t="inlineStr">
@@ -2634,29 +2626,29 @@
       </c>
       <c r="AG13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AH13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AI13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AK13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AL13" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AM13" t="n">
         <v>0</v>
@@ -2664,60 +2656,68 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>262200</v>
+        <v>413401</v>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr"/>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
       <c r="M14" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -2732,37 +2732,37 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AA14" t="inlineStr">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
@@ -2782,7 +2782,7 @@
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AE14" t="inlineStr">
@@ -2792,45 +2792,49 @@
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="AG14" t="inlineStr"/>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
       <c r="AH14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AI14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK14" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AL14" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AM14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>123456</v>
+        <v>261900</v>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2844,12 +2848,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2869,17 +2873,17 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -2889,37 +2893,37 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -2929,7 +2933,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr">
@@ -2939,17 +2943,17 @@
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
@@ -2959,22 +2963,22 @@
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AH15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AI15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ15" t="inlineStr">
@@ -2983,10 +2987,10 @@
         </is>
       </c>
       <c r="AK15" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AL15" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AM15" t="n">
         <v>0</v>
@@ -2994,18 +2998,18 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>993048</v>
+        <v>272500</v>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>1060</v>
+        <v>1071</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -3015,122 +3019,70 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="W16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="X16" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="AB16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="AC16" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="AD16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="AE16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AG16" t="inlineStr">
@@ -3145,451 +3097,639 @@
       </c>
       <c r="AI16" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AJ16" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AK16" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AL16" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="AM16" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> A</t>
-        </is>
-      </c>
+        <v>998586</v>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" t="n">
-        <v>6</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" t="n">
-        <v>2</v>
-      </c>
-      <c r="N17" t="n">
-        <v>2</v>
-      </c>
-      <c r="O17" t="n">
-        <v>3</v>
-      </c>
-      <c r="P17" t="n">
+      <c r="F17" t="n">
+        <v>1071</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AI17" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AK17" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL17" t="n">
         <v>8</v>
       </c>
-      <c r="Q17" t="n">
-        <v>5</v>
-      </c>
-      <c r="R17" t="n">
-        <v>2</v>
-      </c>
-      <c r="S17" t="n">
-        <v>1</v>
-      </c>
-      <c r="T17" t="n">
-        <v>2</v>
-      </c>
-      <c r="U17" t="n">
-        <v>5</v>
-      </c>
-      <c r="V17" t="n">
-        <v>7</v>
-      </c>
-      <c r="W17" t="n">
-        <v>4</v>
-      </c>
-      <c r="X17" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE17" t="n">
-        <v>8</v>
-      </c>
-      <c r="AF17" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG17" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH17" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI17" t="n">
-        <v>11</v>
-      </c>
-      <c r="AJ17" t="n">
-        <v>4</v>
-      </c>
-      <c r="AK17" t="inlineStr"/>
-      <c r="AL17" t="inlineStr"/>
-      <c r="AM17" t="inlineStr"/>
+      <c r="AM17" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> B</t>
-        </is>
-      </c>
+        <v>30193</v>
+      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="n">
-        <v>13</v>
-      </c>
-      <c r="H18" t="n">
-        <v>11</v>
-      </c>
-      <c r="I18" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" t="n">
-        <v>4</v>
-      </c>
-      <c r="L18" t="n">
-        <v>4</v>
-      </c>
-      <c r="M18" t="n">
-        <v>10</v>
-      </c>
-      <c r="N18" t="n">
-        <v>6</v>
-      </c>
-      <c r="O18" t="n">
-        <v>6</v>
-      </c>
-      <c r="P18" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>4</v>
-      </c>
-      <c r="R18" t="n">
-        <v>2</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0</v>
-      </c>
-      <c r="T18" t="n">
-        <v>1</v>
-      </c>
-      <c r="U18" t="n">
-        <v>5</v>
-      </c>
-      <c r="V18" t="n">
-        <v>2</v>
-      </c>
-      <c r="W18" t="n">
-        <v>3</v>
-      </c>
-      <c r="X18" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y18" t="n">
-        <v>7</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA18" t="n">
-        <v>4</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>5</v>
-      </c>
-      <c r="AC18" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD18" t="n">
+      <c r="F18" t="n">
+        <v>1071</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AI18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AK18" t="n">
         <v>8</v>
       </c>
-      <c r="AE18" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG18" t="n">
-        <v>4</v>
-      </c>
-      <c r="AH18" t="n">
-        <v>11</v>
-      </c>
-      <c r="AI18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ18" t="n">
-        <v>6</v>
-      </c>
-      <c r="AK18" t="inlineStr"/>
-      <c r="AL18" t="inlineStr"/>
-      <c r="AM18" t="inlineStr"/>
+      <c r="AL18" t="n">
+        <v>22</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> C</t>
-        </is>
-      </c>
+        <v>281800</v>
+      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" t="n">
-        <v>13</v>
-      </c>
-      <c r="J19" t="n">
-        <v>2</v>
-      </c>
-      <c r="K19" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" t="n">
-        <v>6</v>
-      </c>
-      <c r="M19" t="n">
-        <v>1</v>
-      </c>
-      <c r="N19" t="n">
-        <v>3</v>
-      </c>
-      <c r="O19" t="n">
-        <v>3</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" t="n">
-        <v>2</v>
-      </c>
-      <c r="S19" t="n">
-        <v>13</v>
-      </c>
-      <c r="T19" t="n">
-        <v>1</v>
-      </c>
-      <c r="U19" t="n">
-        <v>1</v>
-      </c>
-      <c r="V19" t="n">
-        <v>3</v>
-      </c>
-      <c r="W19" t="n">
-        <v>6</v>
-      </c>
-      <c r="X19" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>8</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF19" t="n">
-        <v>8</v>
-      </c>
-      <c r="AG19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI19" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ19" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK19" t="inlineStr"/>
-      <c r="AL19" t="inlineStr"/>
-      <c r="AM19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>1071</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AI19" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AK19" t="n">
+        <v>7</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>18</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> D</t>
-        </is>
-      </c>
+        <v>316057</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" t="n">
-        <v>3</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
-        <v>12</v>
-      </c>
-      <c r="K20" t="n">
-        <v>3</v>
-      </c>
-      <c r="L20" t="n">
-        <v>2</v>
-      </c>
-      <c r="M20" t="n">
-        <v>1</v>
-      </c>
-      <c r="N20" t="n">
-        <v>2</v>
-      </c>
-      <c r="O20" t="n">
-        <v>2</v>
-      </c>
-      <c r="P20" t="n">
+      <c r="F20" t="n">
+        <v>1071</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AI20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="AJ20" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="AK20" t="n">
         <v>4</v>
       </c>
-      <c r="Q20" t="n">
-        <v>5</v>
-      </c>
-      <c r="R20" t="n">
-        <v>8</v>
-      </c>
-      <c r="S20" t="n">
-        <v>0</v>
-      </c>
-      <c r="T20" t="n">
-        <v>10</v>
-      </c>
-      <c r="U20" t="n">
-        <v>2</v>
-      </c>
-      <c r="V20" t="n">
-        <v>2</v>
-      </c>
-      <c r="W20" t="n">
-        <v>1</v>
-      </c>
-      <c r="X20" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AG20" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ20" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK20" t="inlineStr"/>
-      <c r="AL20" t="inlineStr"/>
-      <c r="AM20" t="inlineStr"/>
+      <c r="AL20" t="n">
+        <v>26</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -3597,7 +3737,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CORRECT</t>
+          <t xml:space="preserve"> A</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -3605,94 +3745,94 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" t="n">
+        <v>9</v>
+      </c>
+      <c r="J21" t="n">
+        <v>7</v>
+      </c>
+      <c r="K21" t="n">
         <v>11</v>
       </c>
-      <c r="I21" t="n">
-        <v>13</v>
-      </c>
-      <c r="J21" t="n">
-        <v>12</v>
-      </c>
-      <c r="K21" t="n">
-        <v>6</v>
-      </c>
       <c r="L21" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="N21" t="n">
         <v>3</v>
       </c>
       <c r="O21" t="n">
+        <v>3</v>
+      </c>
+      <c r="P21" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>13</v>
+      </c>
+      <c r="R21" t="n">
         <v>6</v>
       </c>
-      <c r="P21" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>5</v>
-      </c>
-      <c r="R21" t="n">
-        <v>8</v>
-      </c>
       <c r="S21" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T21" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="U21" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="W21" t="n">
+        <v>1</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA21" t="n">
         <v>4</v>
       </c>
-      <c r="X21" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>7</v>
-      </c>
-      <c r="Z21" t="n">
+      <c r="AB21" t="n">
         <v>3</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AC21" t="n">
         <v>3</v>
       </c>
-      <c r="AB21" t="n">
-        <v>8</v>
-      </c>
-      <c r="AC21" t="n">
-        <v>5</v>
-      </c>
       <c r="AD21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE21" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AF21" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AG21" t="n">
         <v>5</v>
       </c>
       <c r="AH21" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AI21" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="AJ21" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
@@ -3704,7 +3844,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>INCORRECT</t>
+          <t xml:space="preserve"> B</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -3712,94 +3852,94 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H22" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J22" t="n">
         <v>2</v>
       </c>
       <c r="K22" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M22" t="n">
+        <v>7</v>
+      </c>
+      <c r="N22" t="n">
+        <v>7</v>
+      </c>
+      <c r="O22" t="n">
         <v>4</v>
-      </c>
-      <c r="N22" t="n">
-        <v>10</v>
-      </c>
-      <c r="O22" t="n">
-        <v>8</v>
       </c>
       <c r="P22" t="n">
         <v>6</v>
       </c>
       <c r="Q22" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" t="n">
+        <v>3</v>
+      </c>
+      <c r="T22" t="n">
+        <v>6</v>
+      </c>
+      <c r="U22" t="n">
+        <v>1</v>
+      </c>
+      <c r="V22" t="n">
+        <v>5</v>
+      </c>
+      <c r="W22" t="n">
+        <v>7</v>
+      </c>
+      <c r="X22" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC22" t="n">
         <v>9</v>
       </c>
-      <c r="R22" t="n">
+      <c r="AD22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG22" t="n">
         <v>6</v>
       </c>
-      <c r="S22" t="n">
+      <c r="AH22" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI22" t="n">
         <v>1</v>
       </c>
-      <c r="T22" t="n">
-        <v>4</v>
-      </c>
-      <c r="U22" t="n">
-        <v>8</v>
-      </c>
-      <c r="V22" t="n">
-        <v>7</v>
-      </c>
-      <c r="W22" t="n">
-        <v>10</v>
-      </c>
-      <c r="X22" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>7</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>11</v>
-      </c>
-      <c r="AA22" t="n">
-        <v>11</v>
-      </c>
-      <c r="AB22" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>8</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>11</v>
-      </c>
-      <c r="AE22" t="n">
-        <v>6</v>
-      </c>
-      <c r="AF22" t="n">
-        <v>6</v>
-      </c>
-      <c r="AG22" t="n">
-        <v>7</v>
-      </c>
-      <c r="AH22" t="n">
+      <c r="AJ22" t="n">
         <v>3</v>
-      </c>
-      <c r="AI22" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ22" t="n">
-        <v>8</v>
       </c>
       <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="inlineStr"/>
@@ -3811,7 +3951,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>UNANSWERED</t>
+          <t xml:space="preserve"> C</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -3819,88 +3959,88 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>3</v>
+      </c>
+      <c r="N23" t="n">
+        <v>5</v>
+      </c>
+      <c r="O23" t="n">
+        <v>5</v>
+      </c>
+      <c r="P23" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q23" t="n">
         <v>1</v>
       </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="n">
+      <c r="R23" t="n">
+        <v>5</v>
+      </c>
+      <c r="S23" t="n">
+        <v>2</v>
+      </c>
+      <c r="T23" t="n">
         <v>1</v>
       </c>
-      <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0</v>
-      </c>
-      <c r="S23" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" t="n">
-        <v>0</v>
-      </c>
       <c r="U23" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="V23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W23" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X23" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Y23" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="Z23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AD23" t="n">
         <v>0</v>
       </c>
       <c r="AE23" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AF23" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AG23" t="n">
         <v>2</v>
       </c>
       <c r="AH23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI23" t="n">
         <v>0</v>
@@ -3911,6 +4051,434 @@
       <c r="AK23" t="inlineStr"/>
       <c r="AL23" t="inlineStr"/>
       <c r="AM23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> D</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>7</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2</v>
+      </c>
+      <c r="K24" t="n">
+        <v>3</v>
+      </c>
+      <c r="L24" t="n">
+        <v>16</v>
+      </c>
+      <c r="M24" t="n">
+        <v>5</v>
+      </c>
+      <c r="N24" t="n">
+        <v>2</v>
+      </c>
+      <c r="O24" t="n">
+        <v>3</v>
+      </c>
+      <c r="P24" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1</v>
+      </c>
+      <c r="R24" t="n">
+        <v>3</v>
+      </c>
+      <c r="S24" t="n">
+        <v>1</v>
+      </c>
+      <c r="T24" t="n">
+        <v>4</v>
+      </c>
+      <c r="U24" t="n">
+        <v>2</v>
+      </c>
+      <c r="V24" t="n">
+        <v>4</v>
+      </c>
+      <c r="W24" t="n">
+        <v>2</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>15</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>13</v>
+      </c>
+      <c r="AK24" t="inlineStr"/>
+      <c r="AL24" t="inlineStr"/>
+      <c r="AM24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CORRECT</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>7</v>
+      </c>
+      <c r="H25" t="n">
+        <v>11</v>
+      </c>
+      <c r="I25" t="n">
+        <v>9</v>
+      </c>
+      <c r="J25" t="n">
+        <v>7</v>
+      </c>
+      <c r="K25" t="n">
+        <v>11</v>
+      </c>
+      <c r="L25" t="n">
+        <v>16</v>
+      </c>
+      <c r="M25" t="n">
+        <v>5</v>
+      </c>
+      <c r="N25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O25" t="n">
+        <v>5</v>
+      </c>
+      <c r="P25" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>13</v>
+      </c>
+      <c r="R25" t="n">
+        <v>5</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" t="n">
+        <v>15</v>
+      </c>
+      <c r="V25" t="n">
+        <v>4</v>
+      </c>
+      <c r="W25" t="n">
+        <v>5</v>
+      </c>
+      <c r="X25" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>11</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>15</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>13</v>
+      </c>
+      <c r="AK25" t="inlineStr"/>
+      <c r="AL25" t="inlineStr"/>
+      <c r="AM25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>INCORRECT</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>11</v>
+      </c>
+      <c r="H26" t="n">
+        <v>7</v>
+      </c>
+      <c r="I26" t="n">
+        <v>9</v>
+      </c>
+      <c r="J26" t="n">
+        <v>10</v>
+      </c>
+      <c r="K26" t="n">
+        <v>6</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
+      <c r="M26" t="n">
+        <v>11</v>
+      </c>
+      <c r="N26" t="n">
+        <v>10</v>
+      </c>
+      <c r="O26" t="n">
+        <v>10</v>
+      </c>
+      <c r="P26" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>3</v>
+      </c>
+      <c r="R26" t="n">
+        <v>10</v>
+      </c>
+      <c r="S26" t="n">
+        <v>17</v>
+      </c>
+      <c r="T26" t="n">
+        <v>14</v>
+      </c>
+      <c r="U26" t="n">
+        <v>3</v>
+      </c>
+      <c r="V26" t="n">
+        <v>11</v>
+      </c>
+      <c r="W26" t="n">
+        <v>10</v>
+      </c>
+      <c r="X26" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>15</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>13</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK26" t="inlineStr"/>
+      <c r="AL26" t="inlineStr"/>
+      <c r="AM26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>UNANSWERED</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="n">
+        <v>2</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" t="n">
+        <v>3</v>
+      </c>
+      <c r="P27" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>2</v>
+      </c>
+      <c r="R27" t="n">
+        <v>3</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>3</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>3</v>
+      </c>
+      <c r="W27" t="n">
+        <v>3</v>
+      </c>
+      <c r="X27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="inlineStr"/>
+      <c r="AL27" t="inlineStr"/>
+      <c r="AM27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>